<commit_message>
Changed Lvl 1 formulas so they round to nears whole #
</commit_message>
<xml_diff>
--- a/Stat Spreadsheet.xlsx
+++ b/Stat Spreadsheet.xlsx
@@ -657,7 +657,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,7 +1446,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="3">
-        <f>E29*$D29</f>
+        <f>ROUND(E29*$D29,0)</f>
         <v>70</v>
       </c>
       <c r="G29" s="4">
@@ -1454,7 +1454,7 @@
         <v>0.8</v>
       </c>
       <c r="H29" s="3">
-        <f>G29*$D29</f>
+        <f>ROUND(G29*$D29,0)</f>
         <v>56</v>
       </c>
       <c r="I29" s="4">
@@ -1462,7 +1462,7 @@
         <v>1.2</v>
       </c>
       <c r="J29" s="3">
-        <f>I29*$D29</f>
+        <f>ROUND(I29*$D29,0)</f>
         <v>84</v>
       </c>
       <c r="K29" s="4">
@@ -1470,7 +1470,7 @@
         <v>0.9</v>
       </c>
       <c r="L29" s="3">
-        <f>K29*$D29</f>
+        <f>ROUND(K29*$D29,0)</f>
         <v>63</v>
       </c>
       <c r="M29" s="4">
@@ -1478,7 +1478,7 @@
         <v>0.9</v>
       </c>
       <c r="N29" s="3">
-        <f>M29*$D29</f>
+        <f>ROUND(M29*$D29,0)</f>
         <v>63</v>
       </c>
       <c r="O29" s="4">
@@ -1486,8 +1486,8 @@
         <v>1.08</v>
       </c>
       <c r="P29" s="3">
-        <f>O29*$D29</f>
-        <v>75.600000000000009</v>
+        <f>ROUND(O29*$D29,0)</f>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -1510,7 +1510,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="5">
-        <f t="shared" ref="F30" si="8">E30*$D30</f>
+        <f t="shared" ref="F30:H36" si="8">ROUND(E30*$D30,0)</f>
         <v>0</v>
       </c>
       <c r="G30" s="6">
@@ -1518,7 +1518,7 @@
         <v>1.2</v>
       </c>
       <c r="H30" s="5">
-        <f t="shared" ref="H30" si="10">G30*$D30</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="I30" s="6">
@@ -1526,31 +1526,31 @@
         <v>1.2</v>
       </c>
       <c r="J30" s="5">
-        <f t="shared" ref="J30:J36" si="11">I30*$D30</f>
+        <f t="shared" ref="J30" si="10">ROUND(I30*$D30,0)</f>
         <v>18</v>
       </c>
       <c r="K30" s="6">
-        <f t="shared" ref="K30:L30" si="12">K7</f>
+        <f t="shared" ref="K30:L30" si="11">K7</f>
         <v>1.2</v>
       </c>
       <c r="L30" s="5">
-        <f t="shared" ref="L30:L36" si="13">K30*$D30</f>
+        <f t="shared" ref="L30" si="12">ROUND(K30*$D30,0)</f>
         <v>18</v>
       </c>
       <c r="M30" s="6">
-        <f t="shared" ref="M30:N30" si="14">M7</f>
+        <f t="shared" ref="M30:N30" si="13">M7</f>
         <v>0</v>
       </c>
       <c r="N30" s="5">
-        <f t="shared" ref="N30:N36" si="15">M30*$D30</f>
+        <f t="shared" ref="N30:P30" si="14">ROUND(M30*$D30,0)</f>
         <v>0</v>
       </c>
       <c r="O30" s="6">
-        <f t="shared" ref="O30:P30" si="16">O7</f>
+        <f t="shared" ref="O30:P30" si="15">O7</f>
         <v>0</v>
       </c>
       <c r="P30" s="5">
-        <f t="shared" ref="P30:P36" si="17">O30*$D30</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -1570,52 +1570,52 @@
         <v>15</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" ref="E31" si="18">E8</f>
+        <f t="shared" ref="E31" si="16">E8</f>
         <v>0.95</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" ref="F31" si="19">E31*$D31</f>
-        <v>14.25</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" ref="G31:I31" si="20">G8</f>
+        <f t="shared" ref="G31:I31" si="17">G8</f>
         <v>0.7</v>
       </c>
       <c r="H31" s="3">
-        <f t="shared" ref="H31" si="21">G31*$D31</f>
-        <v>10.5</v>
+        <f t="shared" si="8"/>
+        <v>11</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>0.65</v>
       </c>
       <c r="J31" s="3">
-        <f t="shared" si="11"/>
-        <v>9.75</v>
+        <f t="shared" ref="J31" si="18">ROUND(I31*$D31,0)</f>
+        <v>10</v>
       </c>
       <c r="K31" s="4">
-        <f t="shared" ref="K31:L31" si="22">K8</f>
+        <f t="shared" ref="K31:L31" si="19">K8</f>
         <v>0.8</v>
       </c>
       <c r="L31" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="L31" si="20">ROUND(K31*$D31,0)</f>
         <v>12</v>
       </c>
       <c r="M31" s="4">
-        <f t="shared" ref="M31:N31" si="23">M8</f>
+        <f t="shared" ref="M31:N31" si="21">M8</f>
         <v>1.05</v>
       </c>
       <c r="N31" s="3">
-        <f t="shared" si="15"/>
-        <v>15.75</v>
+        <f t="shared" ref="N31:P31" si="22">ROUND(M31*$D31,0)</f>
+        <v>16</v>
       </c>
       <c r="O31" s="4">
-        <f t="shared" ref="O31:P31" si="24">O8</f>
+        <f t="shared" ref="O31:P31" si="23">O8</f>
         <v>1.1299999999999999</v>
       </c>
       <c r="P31" s="3">
-        <f t="shared" si="17"/>
-        <v>16.95</v>
+        <f t="shared" si="22"/>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -1634,52 +1634,52 @@
         <v>15</v>
       </c>
       <c r="E32" s="6">
-        <f t="shared" ref="E32" si="25">E9</f>
+        <f t="shared" ref="E32" si="24">E9</f>
         <v>0.95</v>
       </c>
       <c r="F32" s="5">
-        <f t="shared" ref="F32" si="26">E32*$D32</f>
-        <v>14.25</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="G32" s="6">
-        <f t="shared" ref="G32:I32" si="27">G9</f>
+        <f t="shared" ref="G32:I32" si="25">G9</f>
         <v>0.75</v>
       </c>
       <c r="H32" s="5">
-        <f t="shared" ref="H32" si="28">G32*$D32</f>
-        <v>11.25</v>
+        <f t="shared" si="8"/>
+        <v>11</v>
       </c>
       <c r="I32" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>0.9</v>
       </c>
       <c r="J32" s="5">
-        <f t="shared" si="11"/>
-        <v>13.5</v>
+        <f t="shared" ref="J32" si="26">ROUND(I32*$D32,0)</f>
+        <v>14</v>
       </c>
       <c r="K32" s="6">
-        <f t="shared" ref="K32:L32" si="29">K9</f>
+        <f t="shared" ref="K32:L32" si="27">K9</f>
         <v>0.8</v>
       </c>
       <c r="L32" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="L32" si="28">ROUND(K32*$D32,0)</f>
         <v>12</v>
       </c>
       <c r="M32" s="6">
-        <f t="shared" ref="M32:N32" si="30">M9</f>
+        <f t="shared" ref="M32:N32" si="29">M9</f>
         <v>0.85</v>
       </c>
       <c r="N32" s="5">
-        <f t="shared" si="15"/>
-        <v>12.75</v>
+        <f t="shared" ref="N32:P32" si="30">ROUND(M32*$D32,0)</f>
+        <v>13</v>
       </c>
       <c r="O32" s="6">
         <f t="shared" ref="O32:P32" si="31">O9</f>
         <v>1.06</v>
       </c>
       <c r="P32" s="5">
-        <f t="shared" si="17"/>
-        <v>15.9</v>
+        <f t="shared" si="30"/>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -1702,31 +1702,31 @@
         <v>0</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" ref="F33" si="33">E33*$D33</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G33" s="4">
-        <f t="shared" ref="G33:I33" si="34">G10</f>
+        <f t="shared" ref="G33:I33" si="33">G10</f>
         <v>1.2</v>
       </c>
       <c r="H33" s="3">
-        <f t="shared" ref="H33" si="35">G33*$D33</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="I33" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>1.05</v>
       </c>
       <c r="J33" s="3">
-        <f t="shared" si="11"/>
-        <v>15.75</v>
+        <f t="shared" ref="J33" si="34">ROUND(I33*$D33,0)</f>
+        <v>16</v>
       </c>
       <c r="K33" s="4">
-        <f t="shared" ref="K33:L33" si="36">K10</f>
+        <f t="shared" ref="K33:L33" si="35">K10</f>
         <v>1.2</v>
       </c>
       <c r="L33" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="L33" si="36">ROUND(K33*$D33,0)</f>
         <v>18</v>
       </c>
       <c r="M33" s="4">
@@ -1734,15 +1734,15 @@
         <v>0</v>
       </c>
       <c r="N33" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="N33:P33" si="38">ROUND(M33*$D33,0)</f>
         <v>0</v>
       </c>
       <c r="O33" s="4">
-        <f t="shared" ref="O33:P33" si="38">O10</f>
+        <f t="shared" ref="O33:P33" si="39">O10</f>
         <v>0</v>
       </c>
       <c r="P33" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
     </row>
@@ -1762,19 +1762,19 @@
         <v>15</v>
       </c>
       <c r="E34" s="6">
-        <f t="shared" ref="E34" si="39">E11</f>
+        <f t="shared" ref="E34" si="40">E11</f>
         <v>0.9</v>
       </c>
       <c r="F34" s="5">
-        <f t="shared" ref="F34" si="40">E34*$D34</f>
-        <v>13.5</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="G34" s="6">
         <f t="shared" ref="G34:I34" si="41">G11</f>
         <v>1.2</v>
       </c>
       <c r="H34" s="5">
-        <f t="shared" ref="H34" si="42">G34*$D34</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="I34" s="6">
@@ -1782,7 +1782,7 @@
         <v>1.2</v>
       </c>
       <c r="J34" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="J34" si="42">ROUND(I34*$D34,0)</f>
         <v>18</v>
       </c>
       <c r="K34" s="6">
@@ -1790,24 +1790,24 @@
         <v>1.05</v>
       </c>
       <c r="L34" s="5">
-        <f t="shared" si="13"/>
-        <v>15.75</v>
+        <f t="shared" ref="L34" si="44">ROUND(K34*$D34,0)</f>
+        <v>16</v>
       </c>
       <c r="M34" s="6">
-        <f t="shared" ref="M34:N34" si="44">M11</f>
+        <f t="shared" ref="M34:N34" si="45">M11</f>
         <v>0.85</v>
       </c>
       <c r="N34" s="5">
-        <f t="shared" si="15"/>
-        <v>12.75</v>
+        <f t="shared" ref="N34:P34" si="46">ROUND(M34*$D34,0)</f>
+        <v>13</v>
       </c>
       <c r="O34" s="6">
-        <f t="shared" ref="O34:P34" si="45">O11</f>
+        <f t="shared" ref="O34:P34" si="47">O11</f>
         <v>0.96</v>
       </c>
       <c r="P34" s="5">
-        <f t="shared" si="17"/>
-        <v>14.399999999999999</v>
+        <f t="shared" si="46"/>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -1826,52 +1826,52 @@
         <v>20</v>
       </c>
       <c r="E35" s="4">
-        <f t="shared" ref="E35" si="46">E12</f>
+        <f t="shared" ref="E35" si="48">E12</f>
         <v>1.08</v>
       </c>
       <c r="F35" s="3">
-        <f t="shared" ref="F35" si="47">E35*$D35</f>
-        <v>21.6</v>
+        <f t="shared" si="8"/>
+        <v>22</v>
       </c>
       <c r="G35" s="4">
-        <f t="shared" ref="G35:I35" si="48">G12</f>
+        <f t="shared" ref="G35:I35" si="49">G12</f>
         <v>1</v>
       </c>
       <c r="H35" s="3">
-        <f t="shared" ref="H35" si="49">G35*$D35</f>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="I35" s="4">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.7</v>
       </c>
       <c r="J35" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="J35" si="50">ROUND(I35*$D35,0)</f>
         <v>14</v>
       </c>
       <c r="K35" s="4">
-        <f t="shared" ref="K35:L35" si="50">K12</f>
+        <f t="shared" ref="K35:L35" si="51">K12</f>
         <v>0.9</v>
       </c>
       <c r="L35" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="L35" si="52">ROUND(K35*$D35,0)</f>
         <v>18</v>
       </c>
       <c r="M35" s="4">
-        <f t="shared" ref="M35:N35" si="51">M12</f>
+        <f t="shared" ref="M35:N35" si="53">M12</f>
         <v>1.2</v>
       </c>
       <c r="N35" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="N35:P35" si="54">ROUND(M35*$D35,0)</f>
         <v>24</v>
       </c>
       <c r="O35" s="4">
-        <f t="shared" ref="O35:P35" si="52">O12</f>
+        <f t="shared" ref="O35:P35" si="55">O12</f>
         <v>0.92</v>
       </c>
       <c r="P35" s="3">
-        <f t="shared" si="17"/>
-        <v>18.400000000000002</v>
+        <f t="shared" si="54"/>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -1890,51 +1890,51 @@
         <v>20</v>
       </c>
       <c r="E36" s="6">
-        <f t="shared" ref="E36" si="53">E13</f>
+        <f t="shared" ref="E36" si="56">E13</f>
         <v>1.1399999999999999</v>
       </c>
       <c r="F36" s="5">
-        <f t="shared" ref="F36" si="54">E36*$D36</f>
-        <v>22.799999999999997</v>
+        <f t="shared" si="8"/>
+        <v>23</v>
       </c>
       <c r="G36" s="6">
-        <f t="shared" ref="G36:I36" si="55">G13</f>
+        <f t="shared" ref="G36:I36" si="57">G13</f>
         <v>1.05</v>
       </c>
       <c r="H36" s="5">
-        <f t="shared" ref="H36" si="56">G36*$D36</f>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="I36" s="6">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="J36" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="J36" si="58">ROUND(I36*$D36,0)</f>
         <v>22</v>
       </c>
       <c r="K36" s="6">
-        <f t="shared" ref="K36:L36" si="57">K13</f>
+        <f t="shared" ref="K36:L36" si="59">K13</f>
         <v>1.1499999999999999</v>
       </c>
       <c r="L36" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="L36" si="60">ROUND(K36*$D36,0)</f>
         <v>23</v>
       </c>
       <c r="M36" s="6">
-        <f t="shared" ref="M36:N36" si="58">M13</f>
+        <f t="shared" ref="M36:N36" si="61">M13</f>
         <v>1.2</v>
       </c>
       <c r="N36" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="N36:P36" si="62">ROUND(M36*$D36,0)</f>
         <v>24</v>
       </c>
       <c r="O36" s="6">
-        <f t="shared" ref="O36:P36" si="59">O13</f>
+        <f t="shared" ref="O36:P36" si="63">O13</f>
         <v>0.9</v>
       </c>
       <c r="P36" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="62"/>
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Slevenel, Time Cave #1 Work
-Added end scene to Slevenel
-Added script which allows you to remember final event locations (after
move routes)
-Time Cave #1 Maps
-Character face graphics for battle
</commit_message>
<xml_diff>
--- a/Stat Spreadsheet.xlsx
+++ b/Stat Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20010" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -905,7 +905,7 @@
   <dimension ref="A1:AF55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="Q6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="S45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="S10" sqref="S10"/>

</xml_diff>

<commit_message>
Started new town, added Digger class
</commit_message>
<xml_diff>
--- a/Stat Spreadsheet.xlsx
+++ b/Stat Spreadsheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="40">
   <si>
     <t>Reminiscence Stat Spreadsheet</t>
   </si>
@@ -133,6 +133,9 @@
   <si>
     <t>Rogue</t>
   </si>
+  <si>
+    <t>Digger</t>
+  </si>
 </sst>
 </file>
 
@@ -565,13 +568,31 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -582,24 +603,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -905,10 +908,10 @@
   <dimension ref="A1:AF55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="S45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="U6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S10" sqref="S10"/>
+      <selection pane="bottomRight" activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,14 +921,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
+      <c r="A1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
     </row>
     <row r="2" spans="1:32" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10"/>
@@ -946,12 +949,12 @@
       <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:32" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="54"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="60"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
@@ -962,66 +965,66 @@
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="51" t="s">
+      <c r="D7" s="56"/>
+      <c r="E7" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49" t="s">
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49" t="s">
+      <c r="H7" s="57"/>
+      <c r="I7" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49" t="s">
+      <c r="J7" s="57"/>
+      <c r="K7" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49" t="s">
+      <c r="L7" s="57"/>
+      <c r="M7" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="49"/>
-      <c r="O7" s="49" t="s">
+      <c r="N7" s="57"/>
+      <c r="O7" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="49" t="s">
+      <c r="P7" s="57"/>
+      <c r="Q7" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R7" s="49"/>
-      <c r="S7" s="49" t="s">
+      <c r="R7" s="57"/>
+      <c r="S7" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="T7" s="49"/>
-      <c r="U7" s="49" t="s">
+      <c r="T7" s="57"/>
+      <c r="U7" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="V7" s="57"/>
+      <c r="W7" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="V7" s="49"/>
-      <c r="W7" s="49" t="s">
+      <c r="X7" s="57"/>
+      <c r="Y7" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="X7" s="49"/>
-      <c r="Y7" s="49" t="s">
+      <c r="Z7" s="57"/>
+      <c r="AA7" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="Z7" s="49"/>
-      <c r="AA7" s="49" t="s">
+      <c r="AB7" s="57"/>
+      <c r="AC7" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="AB7" s="49"/>
-      <c r="AC7" s="49" t="s">
+      <c r="AD7" s="57"/>
+      <c r="AE7" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="AD7" s="49"/>
-      <c r="AE7" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF7" s="49"/>
+      <c r="AF7" s="57"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C8" s="30" t="s">
@@ -1185,11 +1188,11 @@
         <v>6300</v>
       </c>
       <c r="U9" s="16">
-        <v>1</v>
+        <v>1.02</v>
       </c>
       <c r="V9" s="17">
         <f>U9*$D9</f>
-        <v>7000</v>
+        <v>7140</v>
       </c>
       <c r="W9" s="16">
         <v>1</v>
@@ -1297,11 +1300,11 @@
         <v>600</v>
       </c>
       <c r="U10" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V10" s="17">
         <f t="shared" ref="V10:V16" si="7">U10*$D10</f>
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="W10" s="16">
         <v>1</v>
@@ -1409,11 +1412,11 @@
         <v>285</v>
       </c>
       <c r="U11" s="13">
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="V11" s="14">
         <f t="shared" si="7"/>
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="W11" s="13">
         <v>1</v>
@@ -1521,11 +1524,11 @@
         <v>285</v>
       </c>
       <c r="U12" s="13">
-        <v>1</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="V12" s="14">
         <f t="shared" si="7"/>
-        <v>300</v>
+        <v>338.99999999999994</v>
       </c>
       <c r="W12" s="13">
         <v>1</v>
@@ -1633,11 +1636,11 @@
         <v>150</v>
       </c>
       <c r="U13" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V13" s="17">
         <f t="shared" si="7"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="W13" s="16">
         <v>1</v>
@@ -1745,11 +1748,11 @@
         <v>285</v>
       </c>
       <c r="U14" s="16">
-        <v>1</v>
+        <v>0.94</v>
       </c>
       <c r="V14" s="17">
         <f t="shared" si="7"/>
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="W14" s="16">
         <v>1</v>
@@ -1857,11 +1860,11 @@
         <v>520</v>
       </c>
       <c r="U15" s="13">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="V15" s="14">
         <f t="shared" si="7"/>
-        <v>400</v>
+        <v>340</v>
       </c>
       <c r="W15" s="13">
         <v>1</v>
@@ -1969,11 +1972,11 @@
         <v>480</v>
       </c>
       <c r="U16" s="13">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="V16" s="14">
         <f t="shared" si="7"/>
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="W16" s="13">
         <v>1</v>
@@ -2080,7 +2083,7 @@
       </c>
       <c r="U17" s="4">
         <f>SUM(U9:U16)-8</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="V17" s="5" t="s">
         <v>25</v>
@@ -2129,81 +2132,81 @@
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="C21" s="58" t="str">
+      <c r="C21" s="49" t="str">
         <f>C7</f>
         <v>Average</v>
       </c>
-      <c r="D21" s="59"/>
-      <c r="E21" s="60" t="str">
+      <c r="D21" s="50"/>
+      <c r="E21" s="51" t="str">
         <f>E7</f>
         <v>Troublemaker</v>
       </c>
-      <c r="F21" s="51"/>
-      <c r="G21" s="50" t="str">
+      <c r="F21" s="52"/>
+      <c r="G21" s="53" t="str">
         <f>G7</f>
         <v>Scholar</v>
       </c>
-      <c r="H21" s="51"/>
-      <c r="I21" s="50" t="str">
+      <c r="H21" s="52"/>
+      <c r="I21" s="53" t="str">
         <f>I7</f>
         <v>White Mage</v>
       </c>
-      <c r="J21" s="51"/>
-      <c r="K21" s="50" t="str">
+      <c r="J21" s="52"/>
+      <c r="K21" s="53" t="str">
         <f>K7</f>
         <v>Black Mage</v>
       </c>
-      <c r="L21" s="51"/>
-      <c r="M21" s="50" t="str">
+      <c r="L21" s="52"/>
+      <c r="M21" s="53" t="str">
         <f>M7</f>
         <v>Archer</v>
       </c>
-      <c r="N21" s="51"/>
-      <c r="O21" s="50" t="str">
+      <c r="N21" s="52"/>
+      <c r="O21" s="53" t="str">
         <f>O7</f>
         <v>Warrior</v>
       </c>
-      <c r="P21" s="51"/>
-      <c r="Q21" s="50" t="str">
+      <c r="P21" s="52"/>
+      <c r="Q21" s="53" t="str">
         <f>Q7</f>
         <v>Sheep</v>
       </c>
-      <c r="R21" s="51"/>
-      <c r="S21" s="50" t="str">
+      <c r="R21" s="52"/>
+      <c r="S21" s="53" t="str">
         <f>S7</f>
         <v>Rogue</v>
       </c>
-      <c r="T21" s="51"/>
-      <c r="U21" s="50" t="str">
+      <c r="T21" s="52"/>
+      <c r="U21" s="53" t="str">
         <f>U7</f>
-        <v>New Class</v>
-      </c>
-      <c r="V21" s="51"/>
-      <c r="W21" s="50" t="str">
+        <v>Digger</v>
+      </c>
+      <c r="V21" s="52"/>
+      <c r="W21" s="53" t="str">
         <f>W7</f>
         <v>New Class</v>
       </c>
-      <c r="X21" s="51"/>
-      <c r="Y21" s="50" t="str">
+      <c r="X21" s="52"/>
+      <c r="Y21" s="53" t="str">
         <f>Y7</f>
         <v>New Class</v>
       </c>
-      <c r="Z21" s="51"/>
-      <c r="AA21" s="50" t="str">
+      <c r="Z21" s="52"/>
+      <c r="AA21" s="53" t="str">
         <f>AA7</f>
         <v>New Class</v>
       </c>
-      <c r="AB21" s="51"/>
-      <c r="AC21" s="50" t="str">
+      <c r="AB21" s="52"/>
+      <c r="AC21" s="53" t="str">
         <f>AC7</f>
         <v>New Class</v>
       </c>
-      <c r="AD21" s="51"/>
-      <c r="AE21" s="50" t="str">
+      <c r="AD21" s="52"/>
+      <c r="AE21" s="53" t="str">
         <f>AE7</f>
         <v>New Class</v>
       </c>
-      <c r="AF21" s="51"/>
+      <c r="AF21" s="52"/>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C22" s="38" t="s">
@@ -2378,11 +2381,11 @@
       </c>
       <c r="U23" s="16">
         <f t="shared" ref="U23" si="29">U9</f>
-        <v>1</v>
+        <v>1.02</v>
       </c>
       <c r="V23" s="17">
         <f t="shared" si="28"/>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="W23" s="16">
         <f t="shared" ref="W23" si="30">W9</f>
@@ -2506,11 +2509,11 @@
       </c>
       <c r="U24" s="16">
         <f t="shared" ref="U24" si="41">U10</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V24" s="17">
         <f t="shared" si="40"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="W24" s="16">
         <f t="shared" ref="W24" si="42">W10</f>
@@ -2634,11 +2637,11 @@
       </c>
       <c r="U25" s="13">
         <f t="shared" ref="U25" si="53">U11</f>
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="V25" s="14">
         <f t="shared" si="52"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="W25" s="13">
         <f t="shared" ref="W25" si="54">W11</f>
@@ -2762,11 +2765,11 @@
       </c>
       <c r="U26" s="13">
         <f t="shared" ref="U26" si="65">U12</f>
-        <v>1</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="V26" s="14">
         <f t="shared" si="64"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="W26" s="13">
         <f t="shared" ref="W26" si="66">W12</f>
@@ -2890,11 +2893,11 @@
       </c>
       <c r="U27" s="16">
         <f t="shared" ref="U27" si="77">U13</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V27" s="17">
         <f t="shared" si="76"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="W27" s="16">
         <f t="shared" ref="W27" si="78">W13</f>
@@ -3018,11 +3021,11 @@
       </c>
       <c r="U28" s="16">
         <f t="shared" ref="U28" si="89">U14</f>
-        <v>1</v>
+        <v>0.94</v>
       </c>
       <c r="V28" s="17">
         <f t="shared" si="88"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W28" s="16">
         <f t="shared" ref="W28" si="90">W14</f>
@@ -3146,11 +3149,11 @@
       </c>
       <c r="U29" s="13">
         <f t="shared" ref="U29" si="101">U15</f>
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="V29" s="14">
         <f t="shared" si="100"/>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="W29" s="13">
         <f t="shared" ref="W29" si="102">W15</f>
@@ -3274,7 +3277,7 @@
       </c>
       <c r="U30" s="13">
         <f t="shared" ref="U30" si="113">U16</f>
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="V30" s="14">
         <f t="shared" si="112"/>
@@ -3390,7 +3393,7 @@
       </c>
       <c r="U31" s="4">
         <f>SUM(U23:U30)-8</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="V31" s="5" t="s">
         <v>25</v>
@@ -3510,81 +3513,81 @@
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="C46" s="58" t="str">
+      <c r="C46" s="49" t="str">
         <f>C21</f>
         <v>Average</v>
       </c>
-      <c r="D46" s="59"/>
-      <c r="E46" s="60" t="str">
+      <c r="D46" s="50"/>
+      <c r="E46" s="51" t="str">
         <f t="shared" ref="E46" si="123">E21</f>
         <v>Troublemaker</v>
       </c>
-      <c r="F46" s="51"/>
-      <c r="G46" s="50" t="str">
+      <c r="F46" s="52"/>
+      <c r="G46" s="53" t="str">
         <f t="shared" ref="G46" si="124">G21</f>
         <v>Scholar</v>
       </c>
-      <c r="H46" s="51"/>
-      <c r="I46" s="50" t="str">
+      <c r="H46" s="52"/>
+      <c r="I46" s="53" t="str">
         <f t="shared" ref="I46" si="125">I21</f>
         <v>White Mage</v>
       </c>
-      <c r="J46" s="51"/>
-      <c r="K46" s="50" t="str">
+      <c r="J46" s="52"/>
+      <c r="K46" s="53" t="str">
         <f t="shared" ref="K46" si="126">K21</f>
         <v>Black Mage</v>
       </c>
-      <c r="L46" s="51"/>
-      <c r="M46" s="50" t="str">
+      <c r="L46" s="52"/>
+      <c r="M46" s="53" t="str">
         <f t="shared" ref="M46" si="127">M21</f>
         <v>Archer</v>
       </c>
-      <c r="N46" s="51"/>
-      <c r="O46" s="50" t="str">
+      <c r="N46" s="52"/>
+      <c r="O46" s="53" t="str">
         <f t="shared" ref="O46:S46" si="128">O21</f>
         <v>Warrior</v>
       </c>
-      <c r="P46" s="51"/>
-      <c r="Q46" s="50" t="str">
+      <c r="P46" s="52"/>
+      <c r="Q46" s="53" t="str">
         <f t="shared" si="128"/>
         <v>Sheep</v>
       </c>
-      <c r="R46" s="51"/>
-      <c r="S46" s="50" t="str">
+      <c r="R46" s="52"/>
+      <c r="S46" s="53" t="str">
         <f t="shared" si="128"/>
         <v>Rogue</v>
       </c>
-      <c r="T46" s="51"/>
-      <c r="U46" s="50" t="str">
+      <c r="T46" s="52"/>
+      <c r="U46" s="53" t="str">
         <f t="shared" ref="U46" si="129">U21</f>
-        <v>New Class</v>
-      </c>
-      <c r="V46" s="51"/>
-      <c r="W46" s="50" t="str">
+        <v>Digger</v>
+      </c>
+      <c r="V46" s="52"/>
+      <c r="W46" s="53" t="str">
         <f t="shared" ref="W46" si="130">W21</f>
         <v>New Class</v>
       </c>
-      <c r="X46" s="51"/>
-      <c r="Y46" s="50" t="str">
+      <c r="X46" s="52"/>
+      <c r="Y46" s="53" t="str">
         <f t="shared" ref="Y46" si="131">Y21</f>
         <v>New Class</v>
       </c>
-      <c r="Z46" s="51"/>
-      <c r="AA46" s="50" t="str">
+      <c r="Z46" s="52"/>
+      <c r="AA46" s="53" t="str">
         <f t="shared" ref="AA46" si="132">AA21</f>
         <v>New Class</v>
       </c>
-      <c r="AB46" s="51"/>
-      <c r="AC46" s="50" t="str">
+      <c r="AB46" s="52"/>
+      <c r="AC46" s="53" t="str">
         <f t="shared" ref="AC46" si="133">AC21</f>
         <v>New Class</v>
       </c>
-      <c r="AD46" s="51"/>
-      <c r="AE46" s="50" t="str">
+      <c r="AD46" s="52"/>
+      <c r="AE46" s="53" t="str">
         <f t="shared" ref="AE46" si="134">AE21</f>
         <v>New Class</v>
       </c>
-      <c r="AF46" s="51"/>
+      <c r="AF46" s="52"/>
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C47" s="38" t="s">
@@ -3759,11 +3762,11 @@
       </c>
       <c r="U48" s="18">
         <f>V23</f>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="V48" s="17">
         <f>V9</f>
-        <v>7000</v>
+        <v>7140</v>
       </c>
       <c r="W48" s="18">
         <f>X23</f>
@@ -3887,11 +3890,11 @@
       </c>
       <c r="U49" s="18">
         <f t="shared" ref="U49:U55" si="150">V24</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="V49" s="17">
         <f t="shared" si="149"/>
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="W49" s="18">
         <f t="shared" ref="W49:W55" si="151">X24</f>
@@ -4015,11 +4018,11 @@
       </c>
       <c r="U50" s="19">
         <f t="shared" si="150"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="V50" s="14">
         <f t="shared" si="170"/>
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="W50" s="19">
         <f t="shared" si="151"/>
@@ -4143,11 +4146,11 @@
       </c>
       <c r="U51" s="19">
         <f t="shared" si="150"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="V51" s="14">
         <f t="shared" si="185"/>
-        <v>300</v>
+        <v>338.99999999999994</v>
       </c>
       <c r="W51" s="19">
         <f t="shared" si="151"/>
@@ -4271,11 +4274,11 @@
       </c>
       <c r="U52" s="18">
         <f t="shared" si="150"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="V52" s="17">
         <f t="shared" si="200"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="W52" s="18">
         <f t="shared" si="151"/>
@@ -4399,11 +4402,11 @@
       </c>
       <c r="U53" s="18">
         <f t="shared" si="150"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V53" s="17">
         <f t="shared" si="215"/>
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="W53" s="18">
         <f t="shared" si="151"/>
@@ -4527,11 +4530,11 @@
       </c>
       <c r="U54" s="19">
         <f t="shared" si="150"/>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="V54" s="14">
         <f t="shared" si="230"/>
-        <v>400</v>
+        <v>340</v>
       </c>
       <c r="W54" s="19">
         <f t="shared" si="151"/>
@@ -4659,7 +4662,7 @@
       </c>
       <c r="V55" s="14">
         <f t="shared" si="245"/>
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="W55" s="19">
         <f t="shared" si="151"/>
@@ -4704,37 +4707,6 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q46:R46"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="O46:P46"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="S46:T46"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="U46:V46"/>
     <mergeCell ref="AE7:AF7"/>
     <mergeCell ref="AE21:AF21"/>
     <mergeCell ref="AE46:AF46"/>
@@ -4751,6 +4723,37 @@
     <mergeCell ref="Y7:Z7"/>
     <mergeCell ref="Y21:Z21"/>
     <mergeCell ref="Y46:Z46"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S46:T46"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="U46:V46"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q46:R46"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="O46:P46"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="K46:L46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>